<commit_message>
updated voltage table for pac 12kv
</commit_message>
<xml_diff>
--- a/pyMAP/loSim/IMAP_lo_voltage_stepping_table_reduced.xlsx
+++ b/pyMAP/loSim/IMAP_lo_voltage_stepping_table_reduced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonny Woof\Google Drive\Python_packages_woof\pyMAP\pyMAP\loSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2352C189-7A71-4372-A0CE-7372F0881085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1082D287-0697-455C-9F4B-903864F0891E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-11550" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Voltage Table" sheetId="1" r:id="rId1"/>
@@ -689,7 +689,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -724,9 +724,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -764,7 +764,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -870,7 +870,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1012,7 +1012,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2012,37 +2012,37 @@
       </c>
       <c r="C29" s="19">
         <f t="shared" ref="C29:I31" si="12">$H29</f>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="D29" s="20">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="E29" s="20">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="F29" s="20">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="G29" s="20">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="H29" s="21">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="I29" s="20">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="J29" s="42" t="s">
         <v>21</v>
       </c>
       <c r="K29" s="40">
         <f t="shared" ref="K29:K31" si="13">$H29</f>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="M29" s="34"/>
     </row>
@@ -2052,77 +2052,77 @@
       </c>
       <c r="C30" s="1">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="E30" s="3">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="G30" s="3">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="H30" s="15">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="I30" s="3">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="J30" s="43" t="s">
         <v>22</v>
       </c>
       <c r="K30" s="39">
         <f t="shared" si="13"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="M30" s="34"/>
     </row>
-    <row r="31" spans="1:13" ht="13.2">
+    <row r="31" spans="1:13" ht="13.8" thickBot="1">
       <c r="B31" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="D31" s="3">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="E31" s="3">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="G31" s="3">
         <f t="shared" si="12"/>
-        <v>16000</v>
-      </c>
-      <c r="H31" s="15">
-        <v>16000</v>
+        <v>12000</v>
+      </c>
+      <c r="H31" s="17">
+        <v>12000</v>
       </c>
       <c r="I31" s="3">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="J31" s="44" t="s">
         <v>23</v>
       </c>
       <c r="K31" s="39">
         <f t="shared" si="13"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="M31" s="34"/>
     </row>
@@ -2222,31 +2222,31 @@
         <v>4</v>
       </c>
       <c r="C35" s="1">
-        <f>C19*$J35</f>
+        <f t="shared" ref="C35:I46" si="14">C19*$J35</f>
         <v>4000</v>
       </c>
       <c r="D35" s="3">
-        <f>D19*$J35</f>
+        <f t="shared" si="14"/>
         <v>4000</v>
       </c>
       <c r="E35" s="3">
-        <f>E19*$J35</f>
+        <f t="shared" si="14"/>
         <v>4000</v>
       </c>
       <c r="F35" s="3">
-        <f>F19*$J35</f>
+        <f t="shared" si="14"/>
         <v>4000</v>
       </c>
       <c r="G35" s="3">
-        <f>G19*$J35</f>
+        <f t="shared" si="14"/>
         <v>4000</v>
       </c>
       <c r="H35" s="15">
-        <f>H19*$J35</f>
+        <f t="shared" si="14"/>
         <v>4000</v>
       </c>
       <c r="I35" s="18">
-        <f>I19*$J35</f>
+        <f t="shared" si="14"/>
         <v>4000</v>
       </c>
       <c r="J35" s="37">
@@ -2259,31 +2259,31 @@
         <v>5</v>
       </c>
       <c r="C36" s="1">
-        <f>C20*$J36</f>
+        <f t="shared" si="14"/>
         <v>-3500</v>
       </c>
       <c r="D36" s="3">
-        <f>D20*$J36</f>
+        <f t="shared" si="14"/>
         <v>-3500</v>
       </c>
       <c r="E36" s="3">
-        <f>E20*$J36</f>
+        <f t="shared" si="14"/>
         <v>-3500</v>
       </c>
       <c r="F36" s="3">
-        <f>F20*$J36</f>
+        <f t="shared" si="14"/>
         <v>-3500</v>
       </c>
       <c r="G36" s="3">
-        <f>G20*$J36</f>
+        <f t="shared" si="14"/>
         <v>-3500</v>
       </c>
       <c r="H36" s="15">
-        <f>H20*$J36</f>
+        <f t="shared" si="14"/>
         <v>-3500</v>
       </c>
       <c r="I36" s="18">
-        <f>I20*$J36</f>
+        <f t="shared" si="14"/>
         <v>-3500</v>
       </c>
       <c r="J36" s="37">
@@ -2296,31 +2296,31 @@
         <v>6</v>
       </c>
       <c r="C37" s="23">
-        <f>C21*$J37</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D37" s="24">
-        <f>D21*$J37</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E37" s="24">
-        <f>E21*$J37</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F37" s="24">
-        <f>F21*$J37</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G37" s="24">
-        <f>G21*$J37</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H37" s="16">
-        <f>H21*$J37</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I37" s="25">
-        <f>I21*$J37</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J37" s="38">
@@ -2333,31 +2333,31 @@
         <v>7</v>
       </c>
       <c r="C38" s="1">
-        <f>C22*$J38</f>
+        <f t="shared" si="14"/>
         <v>-12.599502109244622</v>
       </c>
       <c r="D38" s="3">
-        <f>D22*$J38</f>
+        <f t="shared" si="14"/>
         <v>-24.301858609591989</v>
       </c>
       <c r="E38" s="3">
-        <f>E22*$J38</f>
+        <f t="shared" si="14"/>
         <v>-46.688299791826964</v>
       </c>
       <c r="F38" s="3">
-        <f>F22*$J38</f>
+        <f t="shared" si="14"/>
         <v>-91.880179718531267</v>
       </c>
       <c r="G38" s="3">
-        <f>G22*$J38</f>
+        <f t="shared" si="14"/>
         <v>-177.17611203052283</v>
       </c>
       <c r="H38" s="15">
-        <f>H22*$J38</f>
+        <f t="shared" si="14"/>
         <v>-362.73217530573254</v>
       </c>
       <c r="I38" s="18">
-        <f>I22*$J38</f>
+        <f t="shared" si="14"/>
         <v>-702.88427269868328</v>
       </c>
       <c r="J38" s="37">
@@ -2373,31 +2373,31 @@
         <v>8</v>
       </c>
       <c r="C39" s="1">
-        <f>C23*$J39</f>
+        <f t="shared" si="14"/>
         <v>-13.652033381647415</v>
       </c>
       <c r="D39" s="3">
-        <f>D23*$J39</f>
+        <f t="shared" si="14"/>
         <v>-26.331975827107986</v>
       </c>
       <c r="E39" s="3">
-        <f>E23*$J39</f>
+        <f t="shared" si="14"/>
         <v>-50.588524988039971</v>
       </c>
       <c r="F39" s="3">
-        <f>F23*$J39</f>
+        <f t="shared" si="14"/>
         <v>-99.555622893129922</v>
       </c>
       <c r="G39" s="3">
-        <f>G23*$J39</f>
+        <f t="shared" si="14"/>
         <v>-191.97696662127987</v>
       </c>
       <c r="H39" s="15">
-        <f>H23*$J39</f>
+        <f t="shared" si="14"/>
         <v>-393.03392490707972</v>
       </c>
       <c r="I39" s="18">
-        <f>I23*$J39</f>
+        <f t="shared" si="14"/>
         <v>-761.60148798869375</v>
       </c>
       <c r="J39" s="37">
@@ -2413,31 +2413,31 @@
         <v>9</v>
       </c>
       <c r="C40" s="1">
-        <f>C24*$J40</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D40" s="3">
-        <f>D24*$J40</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E40" s="3">
-        <f>E24*$J40</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F40" s="3">
-        <f>F24*$J40</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G40" s="3">
-        <f>G24*$J40</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H40" s="15">
-        <f>H24*$J40</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I40" s="18">
-        <f>I24*$J40</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J40" s="37">
@@ -2453,31 +2453,31 @@
         <v>10</v>
       </c>
       <c r="C41" s="1">
-        <f>C25*$J41</f>
+        <f t="shared" si="14"/>
         <v>-2.4994204185132651</v>
       </c>
       <c r="D41" s="3">
-        <f>D25*$J41</f>
+        <f t="shared" si="14"/>
         <v>-4.820869990733164</v>
       </c>
       <c r="E41" s="3">
-        <f>E25*$J41</f>
+        <f t="shared" si="14"/>
         <v>-9.2617699329356338</v>
       </c>
       <c r="F41" s="3">
-        <f>F25*$J41</f>
+        <f t="shared" si="14"/>
         <v>-18.226688265456666</v>
       </c>
       <c r="G41" s="3">
-        <f>G25*$J41</f>
+        <f t="shared" si="14"/>
         <v>-35.147229489089078</v>
       </c>
       <c r="H41" s="15">
-        <f>H25*$J41</f>
+        <f t="shared" si="14"/>
         <v>-71.95682794049992</v>
       </c>
       <c r="I41" s="18">
-        <f>I25*$J41</f>
+        <f t="shared" si="14"/>
         <v>-139.43434334170374</v>
       </c>
       <c r="J41" s="37">
@@ -2493,31 +2493,31 @@
         <v>11</v>
       </c>
       <c r="C42" s="1">
-        <f>C26*$J42</f>
+        <f t="shared" si="14"/>
         <v>27.93083915573661</v>
       </c>
       <c r="D42" s="3">
-        <f>D26*$J42</f>
+        <f t="shared" si="14"/>
         <v>53.872867207342452</v>
       </c>
       <c r="E42" s="3">
-        <f>E26*$J42</f>
+        <f t="shared" si="14"/>
         <v>103.49959709785003</v>
       </c>
       <c r="F42" s="3">
-        <f>F26*$J42</f>
+        <f t="shared" si="14"/>
         <v>203.68189941692279</v>
       </c>
       <c r="G42" s="3">
-        <f>G26*$J42</f>
+        <f t="shared" si="14"/>
         <v>392.76770180722576</v>
       </c>
       <c r="H42" s="15">
-        <f>H26*$J42</f>
+        <f t="shared" si="14"/>
         <v>804.11225437560404</v>
       </c>
       <c r="I42" s="18">
-        <f>I26*$J42</f>
+        <f t="shared" si="14"/>
         <v>1558.1685209163268</v>
       </c>
       <c r="J42" s="37">
@@ -2533,31 +2533,31 @@
         <v>12</v>
       </c>
       <c r="C43" s="1">
-        <f>C27*$J43</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D43" s="3">
-        <f>D27*$J43</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E43" s="3">
-        <f>E27*$J43</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F43" s="3">
-        <f>F27*$J43</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G43" s="3">
-        <f>G27*$J43</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H43" s="15">
-        <f>H27*$J43</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I43" s="18">
-        <f>I27*$J43</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J43" s="37">
@@ -2573,31 +2573,31 @@
         <v>13</v>
       </c>
       <c r="C44" s="1">
-        <f>C28*$J44</f>
+        <f t="shared" si="14"/>
         <v>40.301013668078866</v>
       </c>
       <c r="D44" s="3">
-        <f>D28*$J44</f>
+        <f t="shared" si="14"/>
         <v>77.732399859378575</v>
       </c>
       <c r="E44" s="3">
-        <f>E28*$J44</f>
+        <f t="shared" si="14"/>
         <v>149.33810810422486</v>
       </c>
       <c r="F44" s="3">
-        <f>F28*$J44</f>
+        <f t="shared" si="14"/>
         <v>293.88973838459634</v>
       </c>
       <c r="G44" s="3">
-        <f>G28*$J44</f>
+        <f t="shared" si="14"/>
         <v>566.71897434423784</v>
       </c>
       <c r="H44" s="15">
-        <f>H28*$J44</f>
+        <f t="shared" si="14"/>
         <v>1160.2422245020546</v>
       </c>
       <c r="I44" s="18">
-        <f>I28*$J44</f>
+        <f t="shared" si="14"/>
         <v>2248.2593705288559</v>
       </c>
       <c r="J44" s="37">
@@ -2613,32 +2613,32 @@
         <v>14</v>
       </c>
       <c r="C45" s="19">
-        <f>C29*$J45</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="D45" s="20">
-        <f>D29*$J45</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="E45" s="20">
-        <f>E29*$J45</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="F45" s="20">
-        <f>F29*$J45</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="G45" s="20">
-        <f>G29*$J45</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="H45" s="21">
-        <f>H29*$J45</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="I45" s="22">
-        <f>I29*$J45</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="J45" s="45">
         <v>1</v>
@@ -2653,32 +2653,32 @@
         <v>15</v>
       </c>
       <c r="C46" s="1">
-        <f>C30*$J46</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="D46" s="3">
-        <f>D30*$J46</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="E46" s="3">
-        <f>E30*$J46</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="F46" s="3">
-        <f>F30*$J46</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="G46" s="3">
-        <f>G30*$J46</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="H46" s="15">
-        <f>H30*$J46</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="I46" s="18">
-        <f>I30*$J46</f>
-        <v>16000</v>
+        <f t="shared" si="14"/>
+        <v>12000</v>
       </c>
       <c r="J46" s="37">
         <v>1</v>
@@ -2693,32 +2693,32 @@
         <v>16</v>
       </c>
       <c r="C47" s="23">
-        <f>C29*$J47</f>
-        <v>16000</v>
+        <f t="shared" ref="C47:I47" si="15">C29*$J47</f>
+        <v>12000</v>
       </c>
       <c r="D47" s="24">
-        <f>D29*$J47</f>
-        <v>16000</v>
+        <f t="shared" si="15"/>
+        <v>12000</v>
       </c>
       <c r="E47" s="24">
-        <f>E29*$J47</f>
-        <v>16000</v>
+        <f t="shared" si="15"/>
+        <v>12000</v>
       </c>
       <c r="F47" s="24">
-        <f>F29*$J47</f>
-        <v>16000</v>
+        <f t="shared" si="15"/>
+        <v>12000</v>
       </c>
       <c r="G47" s="24">
-        <f>G29*$J47</f>
-        <v>16000</v>
+        <f t="shared" si="15"/>
+        <v>12000</v>
       </c>
       <c r="H47" s="16">
-        <f>H29*$J47</f>
-        <v>16000</v>
+        <f t="shared" si="15"/>
+        <v>12000</v>
       </c>
       <c r="I47" s="25">
-        <f>I29*$J47</f>
-        <v>16000</v>
+        <f t="shared" si="15"/>
+        <v>12000</v>
       </c>
       <c r="J47" s="38">
         <v>1</v>
@@ -3095,7 +3095,7 @@
         <v>16000</v>
       </c>
       <c r="H61" s="19">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="I61" s="19">
         <v>16000</v>
@@ -3121,7 +3121,7 @@
         <v>16000</v>
       </c>
       <c r="H62" s="1">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="I62" s="1">
         <v>16000</v>
@@ -3147,7 +3147,7 @@
         <v>16000</v>
       </c>
       <c r="H63" s="23">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="I63" s="23">
         <v>16000</v>
@@ -3219,6 +3219,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a834003-1f3f-4d25-9463-7452a5d06d1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7056136A096BB45B68F46439EEB1BEA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5f8cc213d8e2d2c033623cd4eda92ea2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a834003-1f3f-4d25-9463-7452a5d06d1d" xmlns:ns3="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="124341960b286ef0c7dd94412534906a" ns2:_="" ns3:_="">
     <xsd:import namespace="7a834003-1f3f-4d25-9463-7452a5d06d1d"/>
@@ -3447,27 +3467,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6750A1D-6979-4C99-BD24-0D18F36702B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0"/>
+    <ds:schemaRef ds:uri="7a834003-1f3f-4d25-9463-7452a5d06d1d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a834003-1f3f-4d25-9463-7452a5d06d1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D10D99D2-9B69-430E-845C-D0E9593A3303}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C722F93-5C2A-4481-9D5E-56F583B9855C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3484,23 +3503,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D10D99D2-9B69-430E-845C-D0E9593A3303}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6750A1D-6979-4C99-BD24-0D18F36702B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0"/>
-    <ds:schemaRef ds:uri="7a834003-1f3f-4d25-9463-7452a5d06d1d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added load functions for PSPL abm
</commit_message>
<xml_diff>
--- a/pyMAP/loSim/IMAP_lo_voltage_stepping_table_reduced.xlsx
+++ b/pyMAP/loSim/IMAP_lo_voltage_stepping_table_reduced.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonny Woof\Google Drive\Python_packages_woof\pyMAP\pyMAP\loSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1082D287-0697-455C-9F4B-903864F0891E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B2872A-8947-4080-8E23-D0E99C40455A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1626,37 +1626,37 @@
       </c>
       <c r="C19" s="1">
         <f t="shared" ref="C19:I20" si="6">$H19</f>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" si="6"/>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="E19" s="3">
         <f t="shared" si="6"/>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="6"/>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="6"/>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="H19" s="15">
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="I19" s="3">
         <f t="shared" si="6"/>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="J19" s="43" t="s">
         <v>18</v>
       </c>
       <c r="K19" s="39">
         <f t="shared" ref="K19:K20" si="7">$H19</f>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="13.2">
@@ -1665,37 +1665,37 @@
       </c>
       <c r="C20" s="1">
         <f t="shared" si="6"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="D20" s="3">
         <f t="shared" si="6"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="E20" s="3">
         <f t="shared" si="6"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="6"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="6"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="H20" s="15">
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" si="6"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="J20" s="43" t="s">
         <v>19</v>
       </c>
       <c r="K20" s="39">
         <f t="shared" si="7"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.2">
@@ -2223,31 +2223,31 @@
       </c>
       <c r="C35" s="1">
         <f t="shared" ref="C35:I46" si="14">C19*$J35</f>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="D35" s="3">
         <f t="shared" si="14"/>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="E35" s="3">
         <f t="shared" si="14"/>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="14"/>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" si="14"/>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="H35" s="15">
         <f t="shared" si="14"/>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="I35" s="18">
         <f t="shared" si="14"/>
-        <v>4000</v>
+        <v>-3500</v>
       </c>
       <c r="J35" s="37">
         <v>1</v>
@@ -2260,31 +2260,31 @@
       </c>
       <c r="C36" s="1">
         <f t="shared" si="14"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="D36" s="3">
         <f t="shared" si="14"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="E36" s="3">
         <f t="shared" si="14"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="14"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" si="14"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="H36" s="15">
         <f t="shared" si="14"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="I36" s="18">
         <f t="shared" si="14"/>
-        <v>-3500</v>
+        <v>4000</v>
       </c>
       <c r="J36" s="37">
         <v>1</v>
@@ -3230,15 +3230,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7056136A096BB45B68F46439EEB1BEA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5f8cc213d8e2d2c033623cd4eda92ea2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a834003-1f3f-4d25-9463-7452a5d06d1d" xmlns:ns3="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="124341960b286ef0c7dd94412534906a" ns2:_="" ns3:_="">
     <xsd:import namespace="7a834003-1f3f-4d25-9463-7452a5d06d1d"/>
@@ -3467,6 +3458,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6750A1D-6979-4C99-BD24-0D18F36702B5}">
   <ds:schemaRefs>
@@ -3479,14 +3479,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D10D99D2-9B69-430E-845C-D0E9593A3303}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C722F93-5C2A-4481-9D5E-56F583B9855C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3503,4 +3495,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D10D99D2-9B69-430E-845C-D0E9593A3303}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
corrected defl voltage in stepping table
</commit_message>
<xml_diff>
--- a/pyMAP/loSim/IMAP_lo_voltage_stepping_table_reduced.xlsx
+++ b/pyMAP/loSim/IMAP_lo_voltage_stepping_table_reduced.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonny Woof\Google Drive\Python_packages_woof\pyMAP\pyMAP\loSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B2872A-8947-4080-8E23-D0E99C40455A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1199215F-C2FF-4520-B52A-4B937FE98D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="15" spans="1:14" ht="13.2">
       <c r="B15" s="35" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C15" s="19">
         <f t="shared" ref="C15:G15" si="2">$H15</f>
@@ -3219,17 +3219,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a834003-1f3f-4d25-9463-7452a5d06d1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7056136A096BB45B68F46439EEB1BEA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5f8cc213d8e2d2c033623cd4eda92ea2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a834003-1f3f-4d25-9463-7452a5d06d1d" xmlns:ns3="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="124341960b286ef0c7dd94412534906a" ns2:_="" ns3:_="">
     <xsd:import namespace="7a834003-1f3f-4d25-9463-7452a5d06d1d"/>
@@ -3458,6 +3447,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a834003-1f3f-4d25-9463-7452a5d06d1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3468,17 +3468,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6750A1D-6979-4C99-BD24-0D18F36702B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0"/>
-    <ds:schemaRef ds:uri="7a834003-1f3f-4d25-9463-7452a5d06d1d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C722F93-5C2A-4481-9D5E-56F583B9855C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3497,6 +3486,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6750A1D-6979-4C99-BD24-0D18F36702B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0"/>
+    <ds:schemaRef ds:uri="7a834003-1f3f-4d25-9463-7452a5d06d1d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D10D99D2-9B69-430E-845C-D0E9593A3303}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixes implemented to make voltage scaling correct
</commit_message>
<xml_diff>
--- a/pyMAP/loSim/IMAP_lo_voltage_stepping_table_reduced.xlsx
+++ b/pyMAP/loSim/IMAP_lo_voltage_stepping_table_reduced.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonny Woof\Google Drive\Python_packages_woof\pyMAP\pyMAP\loSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1199215F-C2FF-4520-B52A-4B937FE98D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A42FF3-F475-4D08-80BD-007C35E569C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3080,25 +3080,25 @@
         <v>14</v>
       </c>
       <c r="C61" s="19">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="D61" s="19">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="E61" s="19">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="F61" s="19">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="G61" s="19">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="H61" s="19">
         <v>12000</v>
       </c>
       <c r="I61" s="19">
-        <v>16000</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="15.75" customHeight="1">
@@ -3106,25 +3106,25 @@
         <v>15</v>
       </c>
       <c r="C62" s="1">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="D62" s="1">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="E62" s="1">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="F62" s="1">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="G62" s="1">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="H62" s="1">
         <v>12000</v>
       </c>
       <c r="I62" s="1">
-        <v>16000</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="15.75" customHeight="1">
@@ -3132,25 +3132,25 @@
         <v>16</v>
       </c>
       <c r="C63" s="23">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="D63" s="23">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="E63" s="23">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="F63" s="23">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="G63" s="23">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="H63" s="23">
         <v>12000</v>
       </c>
       <c r="I63" s="23">
-        <v>16000</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="13.2">
@@ -3219,6 +3219,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a834003-1f3f-4d25-9463-7452a5d06d1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7056136A096BB45B68F46439EEB1BEA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5f8cc213d8e2d2c033623cd4eda92ea2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a834003-1f3f-4d25-9463-7452a5d06d1d" xmlns:ns3="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="124341960b286ef0c7dd94412534906a" ns2:_="" ns3:_="">
     <xsd:import namespace="7a834003-1f3f-4d25-9463-7452a5d06d1d"/>
@@ -3447,27 +3467,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a834003-1f3f-4d25-9463-7452a5d06d1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D10D99D2-9B69-430E-845C-D0E9593A3303}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6750A1D-6979-4C99-BD24-0D18F36702B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0"/>
+    <ds:schemaRef ds:uri="7a834003-1f3f-4d25-9463-7452a5d06d1d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C722F93-5C2A-4481-9D5E-56F583B9855C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3484,23 +3503,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6750A1D-6979-4C99-BD24-0D18F36702B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9fe4fd8c-7a8f-4612-be0d-62eef2bd99c0"/>
-    <ds:schemaRef ds:uri="7a834003-1f3f-4d25-9463-7452a5d06d1d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D10D99D2-9B69-430E-845C-D0E9593A3303}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>